<commit_message>
Updates after 2024-07-24 procedures.
</commit_message>
<xml_diff>
--- a/Muscle_Response_Times_Exponential_2024_07_24a.xlsx
+++ b/Muscle_Response_Times_Exponential_2024_07_24a.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\MyRepos\NML\Mouse_SCS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCE0EAB0-2E8D-4B27-B0E0-E6BA49B9846A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A660E092-8EEB-4EDF-A374-D72FEFBDF77F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{21034878-75EC-4AEB-A868-4199A65C7D41}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{21034878-75EC-4AEB-A868-4199A65C7D41}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -491,16 +491,16 @@
   <dimension ref="A1:D16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.21875" style="3" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.28515625" style="3" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -514,7 +514,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -528,7 +528,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -542,7 +542,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -556,7 +556,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>16</v>
       </c>
@@ -570,7 +570,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>17</v>
       </c>
@@ -584,7 +584,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -598,7 +598,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -612,35 +612,35 @@
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>8</v>
       </c>
       <c r="B9">
-        <v>7.5000000000000002E-4</v>
+        <v>1E-3</v>
       </c>
       <c r="C9">
-        <v>3.2499999999999999E-3</v>
+        <v>4.0000000000000001E-3</v>
       </c>
       <c r="D9" s="3">
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>9</v>
       </c>
       <c r="B10">
-        <v>7.5000000000000002E-4</v>
+        <v>1E-3</v>
       </c>
       <c r="C10">
-        <v>3.2499999999999999E-3</v>
+        <v>4.0000000000000001E-3</v>
       </c>
       <c r="D10" s="3">
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>10</v>
       </c>
@@ -654,7 +654,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>11</v>
       </c>
@@ -668,7 +668,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>12</v>
       </c>
@@ -682,7 +682,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>13</v>
       </c>
@@ -696,7 +696,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>14</v>
       </c>
@@ -710,7 +710,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>15</v>
       </c>

</xml_diff>